<commit_message>
fix key data, optimiz questions read
</commit_message>
<xml_diff>
--- a/__tests__/test-data/key.xlsx
+++ b/__tests__/test-data/key.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current\image-parsing\__tests__\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\current\image-parsing\__tests__\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>Q1</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>POST</t>
@@ -1031,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BK2" sqref="BK2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,13 +1216,13 @@
         <v>59</v>
       </c>
       <c r="BI1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BJ1" t="s">
         <v>65</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>66</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
@@ -1233,10 +1230,10 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
@@ -1254,106 +1251,106 @@
         <v>62</v>
       </c>
       <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
         <v>60</v>
       </c>
       <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
         <v>61</v>
       </c>
-      <c r="N2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" t="s">
-        <v>63</v>
-      </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S2" t="s">
         <v>61</v>
       </c>
       <c r="T2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" t="s">
         <v>60</v>
       </c>
-      <c r="V2" t="s">
-        <v>60</v>
-      </c>
-      <c r="W2" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AD2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AK2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP2" t="s">
         <v>61</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>62</v>
       </c>
       <c r="AQ2" t="s">
         <v>62</v>
@@ -1365,13 +1362,13 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AU2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AV2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AW2" t="s">
         <v>62</v>
@@ -1380,7 +1377,7 @@
         <v>60</v>
       </c>
       <c r="AY2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AZ2" t="s">
         <v>63</v>
@@ -1392,22 +1389,22 @@
         <v>60</v>
       </c>
       <c r="BC2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF2" t="s">
         <v>60</v>
       </c>
-      <c r="BD2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>63</v>
-      </c>
       <c r="BG2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="BH2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="BI2">
         <v>1</v>

</xml_diff>